<commit_message>
Fallback Excel-Dateine, falls Probleme beim Einlesen der durch ";" getrennten Werte in den .csv-Dateine auftauchen sollten
</commit_message>
<xml_diff>
--- a/data/Feiertage.xlsx
+++ b/data/Feiertage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solsken\Documents\Studium\FH Kiel\SS2020\Projekt_SoSe2020\Application_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC758EC-5669-4E3E-A77A-21CFC2141893}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD25982-D565-46C0-802A-9E9AF9F91D2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34308" yWindow="1344" windowWidth="17280" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B307"/>
+  <dimension ref="A1:B293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:B341"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,7 +429,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>41633</v>
+        <v>41639</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>41634</v>
+        <v>41747</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -445,7 +445,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>41639</v>
+        <v>41749</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>41747</v>
+        <v>41750</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>41749</v>
+        <v>41788</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>41750</v>
+        <v>41798</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>41788</v>
+        <v>41799</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>41798</v>
+        <v>41915</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>41799</v>
+        <v>42004</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>41915</v>
+        <v>42097</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>41998</v>
+        <v>42099</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>41999</v>
+        <v>42100</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>42004</v>
+        <v>42138</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>42097</v>
+        <v>42148</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>42099</v>
+        <v>42149</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>42100</v>
+        <v>42280</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>42138</v>
+        <v>42369</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>42148</v>
+        <v>42454</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>42149</v>
+        <v>42456</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>42280</v>
+        <v>42457</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>42363</v>
+        <v>42495</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>42364</v>
+        <v>42505</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>42369</v>
+        <v>42506</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>42454</v>
+        <v>42646</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>42456</v>
+        <v>42735</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>42457</v>
+        <v>42839</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>42495</v>
+        <v>42841</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>42505</v>
+        <v>42842</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>42506</v>
+        <v>42880</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>42646</v>
+        <v>42890</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>42729</v>
+        <v>42891</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>42730</v>
+        <v>43011</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>42735</v>
+        <v>43100</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>42839</v>
+        <v>43189</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>42841</v>
+        <v>43191</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>42842</v>
+        <v>43192</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>42880</v>
+        <v>43230</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>42890</v>
+        <v>43240</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>42891</v>
+        <v>43241</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>43011</v>
+        <v>43376</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>43094</v>
+        <v>43465</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>43095</v>
+        <v>43574</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>43100</v>
+        <v>43576</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>43189</v>
+        <v>43577</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>43191</v>
+        <v>43615</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>43192</v>
+        <v>43625</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>43230</v>
+        <v>43626</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>43240</v>
+        <v>43741</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -813,149 +813,79 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>43241</v>
+        <v>43830</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>43376</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
+      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>43459</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
+      <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>43460</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
+      <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>43465</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>43574</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>43576</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
+      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>43577</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>43615</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>43625</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>43626</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
-        <v>43741</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>43824</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
-        <v>43825</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
-        <v>43830</v>
-      </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
@@ -1596,48 +1526,6 @@
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="1"/>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A294" s="1"/>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A295" s="1"/>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A296" s="1"/>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A297" s="1"/>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A298" s="1"/>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A299" s="1"/>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A300" s="1"/>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A301" s="1"/>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A302" s="1"/>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A303" s="1"/>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A304" s="1"/>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A305" s="1"/>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A306" s="1"/>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A307" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>